<commit_message>
allocate image address & add image_info.vhd
</commit_message>
<xml_diff>
--- a/docs/sram_alloc.xlsx
+++ b/docs/sram_alloc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>backgroud2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>help</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,6 +115,10 @@
   </si>
   <si>
     <t>address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>background2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,7 +445,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D2:D18"/>
+      <selection activeCell="E4" sqref="E4:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -455,304 +455,379 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="C2">
         <v>480</v>
       </c>
       <c r="D2">
-        <f>B2*C2</f>
-        <v>153600</v>
+        <f t="shared" ref="D2:D3" si="0">B2*C2</f>
+        <v>307200</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="C3">
         <v>480</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D20" si="0">B3*C3</f>
-        <v>153600</v>
+        <f t="shared" si="0"/>
+        <v>307200</v>
+      </c>
+      <c r="E3">
+        <f>E2+D2</f>
+        <v>307200</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>252</v>
+        <v>320</v>
       </c>
       <c r="C4">
-        <v>105</v>
+        <v>480</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>26460</v>
+        <f>B4*C4</f>
+        <v>153600</v>
+      </c>
+      <c r="E4">
+        <f>E3+D3</f>
+        <v>614400</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>72</v>
+        <v>320</v>
       </c>
       <c r="C5">
-        <v>70</v>
+        <v>480</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>5040</v>
+        <f t="shared" ref="D5:D22" si="1">B5*C5</f>
+        <v>153600</v>
+      </c>
+      <c r="E5">
+        <f>E4+ROUNDUP(D4/2,0)</f>
+        <v>691200</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="C6">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1980</v>
+        <f t="shared" si="1"/>
+        <v>26460</v>
+      </c>
+      <c r="E6">
+        <f>E5+ROUNDUP(D5/2,0)</f>
+        <v>768000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="C7">
-        <v>285</v>
+        <v>70</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>46455</v>
+        <f t="shared" si="1"/>
+        <v>5040</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E20" si="2">E6+ROUNDUP(D6/2,0)</f>
+        <v>781230</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>211</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>24476</v>
+        <f t="shared" si="1"/>
+        <v>1980</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>783750</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="C9">
-        <v>209</v>
+        <v>285</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>22781</v>
+        <f t="shared" si="1"/>
+        <v>46455</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>784740</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>24600</v>
+        <f t="shared" si="1"/>
+        <v>24476</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>807968</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C11">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>19809</v>
+        <f t="shared" si="1"/>
+        <v>22781</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>820206</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C12">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>23326</v>
+        <f t="shared" si="1"/>
+        <v>24600</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>831597</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C13">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>23108</v>
+        <f t="shared" si="1"/>
+        <v>19809</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>843897</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C14">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>27032</v>
+        <f t="shared" si="1"/>
+        <v>23326</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>853802</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C15">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>27625</v>
+        <f t="shared" si="1"/>
+        <v>23108</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>865465</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>124</v>
+      </c>
+      <c r="C16">
+        <v>218</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>27032</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>877019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>125</v>
+      </c>
+      <c r="C17">
+        <v>221</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>27625</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>890535</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>122</v>
+      </c>
+      <c r="C18">
+        <v>216</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>26352</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>904348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>122</v>
-      </c>
-      <c r="C16">
-        <v>216</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>26352</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+      <c r="B19">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>1012</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>917524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>44</v>
-      </c>
-      <c r="C17">
-        <v>23</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
+      <c r="B20">
         <v>290</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>121</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
+      <c r="D20">
+        <f t="shared" si="1"/>
         <v>35090</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>640</v>
-      </c>
-      <c r="C19">
-        <v>480</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>307200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>640</v>
-      </c>
-      <c r="C20">
-        <v>480</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>307200</v>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>918030</v>
       </c>
     </row>
   </sheetData>

</xml_diff>